<commit_message>
Docs : WeaponDB_Sheet 수정
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/MeleeWeaponDB_Sheet.xlsx
+++ b/Assets/Excel/Items/MeleeWeaponDB_Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87252289-1596-4DD9-9933-9D1D10E06637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9031F533-CE2E-4A3B-822B-9CDFD971C729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1410" windowWidth="28800" windowHeight="15345" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
+    <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{064CB631-03A8-40F1-A978-87CA5E6CA866}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,96 +27,83 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
-    <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Icon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconWidth</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IconHeight</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Prefab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Axe</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발등 조심하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Icons/Weapons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resources/Prefabs/Weapons</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spear</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>창</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Melee</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>itemName</t>
+  </si>
+  <si>
+    <t>description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>icon</t>
+  </si>
+  <si>
+    <t>iconWidth</t>
+  </si>
+  <si>
+    <t>iconHeight</t>
+  </si>
+  <si>
+    <t>itemPrefab</t>
   </si>
   <si>
     <t>price</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Atk</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtkRate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CritRate</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CritDamage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Range</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LifeSteal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>WeaponTier</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Axe</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>발등 안찍히도록 조심하세요.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resources/Items/Icons/Weapon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resources/Items/Prefabs/Weapons/</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Melee</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Spear</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>창.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>atk</t>
+  </si>
+  <si>
+    <t>atkRate</t>
+  </si>
+  <si>
+    <t>critRate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>critDamage</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>lifeSteal</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>weaponTier</t>
   </si>
 </sst>
 </file>
@@ -482,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{473E7DDB-F7BE-402A-B284-D6385005C611}">
   <dimension ref="A1:P3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:R3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -501,52 +488,52 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -554,13 +541,13 @@
         <v>110001</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -569,7 +556,7 @@
         <v>2</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H2">
         <v>24</v>
@@ -581,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="K2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -593,7 +580,7 @@
         <v>1</v>
       </c>
       <c r="O2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -604,13 +591,13 @@
         <v>110011</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -619,7 +606,7 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>30</v>
@@ -631,7 +618,7 @@
         <v>0.7</v>
       </c>
       <c r="K3">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -640,10 +627,10 @@
         <v>4</v>
       </c>
       <c r="N3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O3" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="P3">
         <v>1</v>

</xml_diff>